<commit_message>
update result of 3 counties
</commit_message>
<xml_diff>
--- a/Presentation/Results.xlsx
+++ b/Presentation/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Model</t>
   </si>
@@ -107,6 +107,32 @@
   </si>
   <si>
     <t>0.06659334</t>
+  </si>
+  <si>
+    <t>LASSO w/o outliers, w/ transformed variables, 3 counties</t>
+  </si>
+  <si>
+    <t>0.04226254</t>
+  </si>
+  <si>
+    <t>0.0004585703, 0.001025403, 0.0001724684</t>
+  </si>
+  <si>
+    <t>bestlam.6059, 
+bestlam.6111,
+bestlam.other</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0.06661122</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>overfit on 6111</t>
   </si>
 </sst>
 </file>
@@ -190,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -203,8 +229,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +565,7 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -556,116 +594,134 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>42980</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="H2" s="10"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>42980</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="H3" s="10"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>42980</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>42980</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>42980</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>42980</v>
       </c>
@@ -678,7 +734,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>42980</v>
       </c>
@@ -691,7 +747,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42980</v>
       </c>
@@ -704,7 +760,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42980</v>
       </c>
@@ -717,7 +773,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -727,7 +783,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -737,7 +793,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -747,7 +803,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -757,7 +813,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -767,7 +823,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
lasso model with zoning
</commit_message>
<xml_diff>
--- a/Presentation/Results.xlsx
+++ b/Presentation/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Model</t>
   </si>
@@ -161,6 +161,62 @@
   </si>
   <si>
     <t>0.0650638</t>
+  </si>
+  <si>
+    <t>Simple XGBoost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">param &lt;- list(objective           = "reg:linear",
+              eval_metric         = "mae",
+              eta                 = 0.037,
+              max_depth           = 5, 
+              subsample           = 0.8,
+              colsample_bytree    = 0.5,
+              min_child_weight    = 4,
+              maximize            = FALSE,
+              lambda              = 0.8,
+              alpha               = 0.4,
+              base_score          = y_mean,
+              silent              = 0)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgb_cv &lt;- xgb.cv(data = x.train,
+                 label = y.train,
+                 params = param,
+                 nrounds = 1000,
+                 prediction = TRUE,
+                 maximize = FALSE,
+                 nfold = 5,
+                 print_every_n = 5)
+</t>
+  </si>
+  <si>
+    <t>0.0419984 ± 0.0004270834</t>
+  </si>
+  <si>
+    <t>0.06629644</t>
+  </si>
+  <si>
+    <t>0.04052988</t>
+  </si>
+  <si>
+    <t>0.04036077</t>
+  </si>
+  <si>
+    <t>LASSO w/o outliers (0.2) and transformed variables, with zoniers</t>
+  </si>
+  <si>
+    <t>lambda = 0.0001883859</t>
+  </si>
+  <si>
+    <t>0.04213434</t>
+  </si>
+  <si>
+    <t>0.04217764 ± 0.0001447036</t>
+  </si>
+  <si>
+    <t>0.06666003</t>
   </si>
 </sst>
 </file>
@@ -191,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +269,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -260,20 +328,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,125 +704,125 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="11">
         <v>42980</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>42980</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="11">
         <v>42980</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="11">
         <v>42980</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="11">
         <v>42980</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="1" t="s">
         <v>37</v>
       </c>
@@ -755,26 +831,26 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="12">
         <v>42981</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -782,35 +858,57 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>42981</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" s="12">
+        <v>42982</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>42981</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="12">
+        <v>42987</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>42981</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>

</xml_diff>

<commit_message>
XGB with zoning test
</commit_message>
<xml_diff>
--- a/Presentation/Results.xlsx
+++ b/Presentation/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Model</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>0.06666003</t>
+  </si>
+  <si>
+    <t>Simple XGBoost with zoning</t>
+  </si>
+  <si>
+    <t>0.04046207</t>
+  </si>
+  <si>
+    <t>0.06641165</t>
+  </si>
+  <si>
+    <t>0.0402112 ±9.030482e-05</t>
   </si>
 </sst>
 </file>
@@ -312,12 +324,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -654,15 +665,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -674,251 +685,267 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>42980</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="H2" s="9"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>42980</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="H3" s="9"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>42980</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>42980</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>42980</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+    <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>42981</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>44</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+    <row r="8" spans="1:11" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>42982</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>42987</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+    <row r="10" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>42982</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -928,7 +955,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -938,7 +965,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -948,7 +975,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -958,7 +985,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -968,7 +995,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -978,7 +1005,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -988,7 +1015,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -998,7 +1025,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1008,7 +1035,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1018,7 +1045,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1028,7 +1055,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1038,7 +1065,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1048,7 +1075,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1058,7 +1085,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1068,7 +1095,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1078,7 +1105,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1088,7 +1115,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1098,7 +1125,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1108,7 +1135,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1118,7 +1145,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1128,7 +1155,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1138,7 +1165,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1148,7 +1175,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1158,7 +1185,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1168,7 +1195,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1178,7 +1205,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
update catboost by cities
</commit_message>
<xml_diff>
--- a/Presentation/Results.xlsx
+++ b/Presentation/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Model</t>
   </si>
@@ -281,7 +281,10 @@
     <t>0.04274147</t>
   </si>
   <si>
-    <t>0.04244559</t>
+    <t>0.0646235</t>
+  </si>
+  <si>
+    <t>0.04063618</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1061,9 +1064,11 @@
         <v>69</v>
       </c>
       <c r="H13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>

</xml_diff>